<commit_message>
finished ldap username with prefix
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/UserdirectoryBundle/Util/users.xlsx
+++ b/Scanorders2/src/Oleg/UserdirectoryBundle/Util/users.xlsx
@@ -10,7 +10,7 @@
     <sheet name="owssvr.dll" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="owssvr.dll" localSheetId="0" hidden="1">owssvr.dll!$A$1:$O$174</definedName>
+    <definedName name="owssvr.dll" localSheetId="0" hidden="1">owssvr.dll!$A$1:$O$173</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="971">
   <si>
     <t>A</t>
   </si>
@@ -2938,15 +2938,6 @@
   </si>
   <si>
     <t>C-312</t>
-  </si>
-  <si>
-    <t>Oleg</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>oli2002@med.cornell.edu</t>
   </si>
 </sst>
 </file>
@@ -3588,8 +3579,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:O174" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:O174"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:O173" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:O173"/>
   <tableColumns count="15">
     <tableColumn id="1" uniqueName="A" name="A" queryTableFieldId="1" dataDxfId="14"/>
     <tableColumn id="2" uniqueName="Primary_x005f_x0020_Group" name="Primary Group" queryTableFieldId="2" dataDxfId="13"/>
@@ -3866,7 +3857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3874,10 +3865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O174"/>
+  <dimension ref="A1:O173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G159" workbookViewId="0">
-      <selection activeCell="O174" sqref="O174"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11363,37 +11354,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
-      <c r="B174" s="2"/>
-      <c r="C174" s="3"/>
-      <c r="D174" s="2"/>
-      <c r="E174" s="2"/>
-      <c r="F174" s="2"/>
-      <c r="G174" s="2" t="s">
-        <v>971</v>
-      </c>
-      <c r="H174" s="2" t="s">
-        <v>972</v>
-      </c>
-      <c r="I174" s="2"/>
-      <c r="J174" s="2"/>
-      <c r="K174" s="2"/>
-      <c r="L174" s="4" t="s">
-        <v>973</v>
-      </c>
-      <c r="M174" s="2"/>
-      <c r="N174" s="2"/>
-      <c r="O174" s="2"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L174" r:id="rId1"/>
-    <hyperlink ref="L173" r:id="rId2"/>
+    <hyperlink ref="L173" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
testing scan and user forms
</commit_message>
<xml_diff>
--- a/Scanorders2/src/Oleg/UserdirectoryBundle/Util/users.xlsx
+++ b/Scanorders2/src/Oleg/UserdirectoryBundle/Util/users.xlsx
@@ -10,7 +10,7 @@
     <sheet name="owssvr.dll" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="owssvr.dll" localSheetId="0" hidden="1">owssvr.dll!$A$1:$O$174</definedName>
+    <definedName name="owssvr.dll" localSheetId="0" hidden="1">owssvr.dll!$A$1:$O$173</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2090" uniqueCount="971">
   <si>
     <t>A</t>
   </si>
@@ -2935,21 +2935,6 @@
   </si>
   <si>
     <t>C-312</t>
-  </si>
-  <si>
-    <t>Oleg Ivanov</t>
-  </si>
-  <si>
-    <t>Ivanov</t>
-  </si>
-  <si>
-    <t>Oleg</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>oli2002@med.cornell.edu</t>
   </si>
   <si>
     <t>Pathology informatics</t>
@@ -3594,8 +3579,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:O174" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:O174"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_owssvr.dll" displayName="Table_owssvr.dll" ref="A1:O173" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:O173"/>
   <tableColumns count="15">
     <tableColumn id="1" uniqueName="A" name="A" queryTableFieldId="1" dataDxfId="14"/>
     <tableColumn id="2" uniqueName="Primary_x005f_x0020_Group" name="Primary Group" queryTableFieldId="2" dataDxfId="13"/>
@@ -3872,7 +3857,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3880,10 +3865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O174"/>
+  <dimension ref="A1:O173"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C174" sqref="C174"/>
+      <selection activeCell="H177" sqref="H177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4558,7 +4543,7 @@
         <v>91</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>975</v>
+        <v>970</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
@@ -6117,7 +6102,7 @@
         <v>300</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>975</v>
+        <v>970</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
@@ -6244,7 +6229,7 @@
         <v>300</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>975</v>
+        <v>970</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
@@ -11369,44 +11354,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
-      <c r="B174" s="2"/>
-      <c r="C174" s="3" t="s">
-        <v>975</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>970</v>
-      </c>
-      <c r="E174" s="2"/>
-      <c r="F174" s="2" t="s">
-        <v>971</v>
-      </c>
-      <c r="G174" s="2" t="s">
-        <v>972</v>
-      </c>
-      <c r="H174" s="2" t="s">
-        <v>973</v>
-      </c>
-      <c r="I174" s="2"/>
-      <c r="J174" s="2"/>
-      <c r="K174" s="2"/>
-      <c r="L174" s="4" t="s">
-        <v>974</v>
-      </c>
-      <c r="M174" s="2"/>
-      <c r="N174" s="2"/>
-      <c r="O174" s="2"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L173" r:id="rId1"/>
-    <hyperlink ref="L174" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>